<commit_message>
trying github and eclipse
</commit_message>
<xml_diff>
--- a/Documents/Test Designs.xlsx
+++ b/Documents/Test Designs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00290732\Documents\GitHub\SoftwareEngineeringGroup\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ciara\Documents\GitHub\SoftwareEngineeringGroup\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D65BB2E-15CB-4FCA-9CC7-65D7D8D5B26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5756784E-2AD7-4CF1-8937-3581BE14FE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" xr2:uid="{5A776C0D-4F55-48DC-9152-FD2EB1331C22}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5A776C0D-4F55-48DC-9152-FD2EB1331C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Publications" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="79">
   <si>
     <t>Test Number</t>
   </si>
@@ -74,9 +74,6 @@
     <t>4. Declare test pass or fail</t>
   </si>
   <si>
-    <t>Verfy negative publications ID entered displays error message</t>
-  </si>
-  <si>
     <t>publicationID = -1536</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>Verify publication ID not entered displays error message</t>
   </si>
   <si>
-    <t xml:space="preserve">publivationID = null </t>
-  </si>
-  <si>
     <t>Fault message: "Error, publicaton ID cannot be left empty"</t>
   </si>
   <si>
@@ -234,6 +228,51 @@
   </si>
   <si>
     <t>"Publication frequency entered succesfully"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUnit </t>
+  </si>
+  <si>
+    <t>pubType = Blog/Journal</t>
+  </si>
+  <si>
+    <t>Fault message: "Error, invalid publication type"</t>
+  </si>
+  <si>
+    <t>Verify invalid inputs displays error message</t>
+  </si>
+  <si>
+    <t>Verify empty publication type displays error message</t>
+  </si>
+  <si>
+    <t>pubType = ""</t>
+  </si>
+  <si>
+    <t>Fault message: "Error, publication type cannot be left empty"</t>
+  </si>
+  <si>
+    <t>Verify invalid frequency dipslays error message</t>
+  </si>
+  <si>
+    <t>pubFrequency = today/ tomorrow</t>
+  </si>
+  <si>
+    <t>Fault message: "Error, invalid frequency entered"</t>
+  </si>
+  <si>
+    <t>Verify empty frequency displays error message</t>
+  </si>
+  <si>
+    <t>pubFrequency = ""</t>
+  </si>
+  <si>
+    <t>Fault message: "Error, frequency cannot be left empty"</t>
+  </si>
+  <si>
+    <t>Verify negative publications ID entered displays error message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">publicationID = null </t>
   </si>
 </sst>
 </file>
@@ -290,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -303,12 +342,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -331,9 +364,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -371,7 +404,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -477,7 +510,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,7 +652,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,26 +665,26 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="43.81640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="46" style="2" customWidth="1"/>
-    <col min="6" max="6" width="55.42578125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="55.453125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="3">
         <v>1</v>
       </c>
       <c r="C1" s="3">
@@ -664,7 +697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -672,33 +705,33 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -706,16 +739,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -723,18 +756,18 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -749,7 +782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -763,7 +796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
@@ -777,7 +810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
@@ -791,7 +824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,78 +841,78 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>20</v>
+      <c r="B13" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
@@ -893,7 +926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
@@ -907,7 +940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
@@ -921,7 +954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
@@ -935,19 +968,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,89 +1000,89 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>9</v>
@@ -1067,7 +1100,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
@@ -1084,7 +1117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1101,7 +1134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>11</v>
       </c>
@@ -1118,7 +1151,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -1129,185 +1162,281 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B59" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B60" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1327,7 +1456,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1342,7 +1471,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Customer Test Design + UML Update
Added tests to customer sheet in test spreadsheet. Updated Customer class skeleton doc to better reflect system architecture
</commit_message>
<xml_diff>
--- a/Documents/Test Designs.xlsx
+++ b/Documents/Test Designs.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00290732\Documents\GitHub\SoftwareEngineeringGroup\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captain\Documents\GitHub\SoftwareEngineeringGroup\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D65BB2E-15CB-4FCA-9CC7-65D7D8D5B26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DA652B-DAA1-4179-BBA7-FAC23267DC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" xr2:uid="{5A776C0D-4F55-48DC-9152-FD2EB1331C22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5A776C0D-4F55-48DC-9152-FD2EB1331C22}"/>
   </bookViews>
   <sheets>
-    <sheet name="Publications" sheetId="4" r:id="rId1"/>
-    <sheet name="Customer" sheetId="2" r:id="rId2"/>
-    <sheet name="Delivry Area" sheetId="3" r:id="rId3"/>
+    <sheet name="Customer" sheetId="2" r:id="rId1"/>
+    <sheet name="Delivery Area" sheetId="3" r:id="rId2"/>
+    <sheet name="Publications" sheetId="4" r:id="rId3"/>
+    <sheet name="Order" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="124">
   <si>
     <t>Test Number</t>
   </si>
@@ -234,13 +235,187 @@
   </si>
   <si>
     <t>"Publication frequency entered succesfully"</t>
+  </si>
+  <si>
+    <t>Check maximum first name</t>
+  </si>
+  <si>
+    <t>JUnit</t>
+  </si>
+  <si>
+    <t>"fnthrdsfytunmightjkiw" (21 char)</t>
+  </si>
+  <si>
+    <t>1. Run Junit test case with given input against validateFirstName()</t>
+  </si>
+  <si>
+    <t>2.Observe results</t>
+  </si>
+  <si>
+    <t>3. Test passes if validateFirstName() returns false</t>
+  </si>
+  <si>
+    <t>Check short first name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"E" </t>
+  </si>
+  <si>
+    <t>1. Run test case with given input as parameter for validateFirstName()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Observe result </t>
+  </si>
+  <si>
+    <t>Check valid first name not rejected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUnit </t>
+  </si>
+  <si>
+    <t>"John"</t>
+  </si>
+  <si>
+    <t>2. Observe result</t>
+  </si>
+  <si>
+    <t>3. Test passes if validateFirstName() returns true</t>
+  </si>
+  <si>
+    <t>Check that number inputs are rejected</t>
+  </si>
+  <si>
+    <t>"S4oirse"</t>
+  </si>
+  <si>
+    <t>1. Run test case with above input as a paramter for validateFirstName()</t>
+  </si>
+  <si>
+    <t>2. Observe</t>
+  </si>
+  <si>
+    <t>3. Test case passes if validateFirstName() returns false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Procedure </t>
+  </si>
+  <si>
+    <t>Test Procedure</t>
+  </si>
+  <si>
+    <t>Check maximum last name</t>
+  </si>
+  <si>
+    <t>"kgjtyardfrtynbfrygkmle" (22 char)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"K" </t>
+  </si>
+  <si>
+    <t>"Murphy"</t>
+  </si>
+  <si>
+    <t>Check valid surname not rejected</t>
+  </si>
+  <si>
+    <t>Check short surname</t>
+  </si>
+  <si>
+    <t>"K3nnedy"</t>
+  </si>
+  <si>
+    <t>1. Run test case with above input as a paramter for validateLastName()</t>
+  </si>
+  <si>
+    <t>1. Run test case with given input as parameter for validatelastName()</t>
+  </si>
+  <si>
+    <t>3. Test case passes if validateLastName() returns false</t>
+  </si>
+  <si>
+    <t>1. Run Junit test case with given input against validateLastName()</t>
+  </si>
+  <si>
+    <t>Check valid eircodes are accepted</t>
+  </si>
+  <si>
+    <t>"N37N6P6"</t>
+  </si>
+  <si>
+    <t>1. Run test case with the above input passed into validateEircode()</t>
+  </si>
+  <si>
+    <t>2. Observe Result</t>
+  </si>
+  <si>
+    <t>3. Test passes if validateEircode returns true</t>
+  </si>
+  <si>
+    <t>Check short eircodes are rejected</t>
+  </si>
+  <si>
+    <t>"D01K3"</t>
+  </si>
+  <si>
+    <t>Check long eircodes are rejected</t>
+  </si>
+  <si>
+    <t>"D01K4H789"</t>
+  </si>
+  <si>
+    <t>2. observe result</t>
+  </si>
+  <si>
+    <t>3. Test passes if validateEircode() returns false</t>
+  </si>
+  <si>
+    <t>Check format is accounted for</t>
+  </si>
+  <si>
+    <t>"1234567"</t>
+  </si>
+  <si>
+    <t>Test Complete</t>
+  </si>
+  <si>
+    <t>Check valid phone numbers are accepted</t>
+  </si>
+  <si>
+    <t>1. Run test case with the above input passed into validatePhoneNo()</t>
+  </si>
+  <si>
+    <t>3. Test passes if validatePhoneNo() returns true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"0861234567" </t>
+  </si>
+  <si>
+    <t>Check short inputs are rejected</t>
+  </si>
+  <si>
+    <t>"083123"</t>
+  </si>
+  <si>
+    <t>3. Test passes if validatePhoneNo() returns false</t>
+  </si>
+  <si>
+    <t>Check long inputs are rejected</t>
+  </si>
+  <si>
+    <t>"083123456789"</t>
+  </si>
+  <si>
+    <t>Check letters are rejected as phone number inputs</t>
+  </si>
+  <si>
+    <t>"wervghjmki"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +444,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -278,7 +461,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -286,11 +469,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -304,17 +506,100 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,10 +615,27 @@
 </styleSheet>
 </file>
 
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -371,7 +673,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -477,7 +779,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,21 +921,713 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3A4903-353E-4552-8E0F-D25A39E4E38B}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="6">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="6">
+        <v>9</v>
+      </c>
+      <c r="C21" s="6">
+        <v>10</v>
+      </c>
+      <c r="D21" s="6">
+        <v>11</v>
+      </c>
+      <c r="E21" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="6">
+        <v>13</v>
+      </c>
+      <c r="C31" s="6">
+        <v>14</v>
+      </c>
+      <c r="D31" s="6">
+        <v>15</v>
+      </c>
+      <c r="E31" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="27"/>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="27"/>
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="27"/>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="27"/>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A26:A28"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:E3 B13:E13" xr:uid="{08C0B9E7-F756-44D9-BFAA-42336D460A9D}">
+      <formula1>"JUnit, UAT"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:E23" xr:uid="{DA8F7369-C690-4CCF-9578-85896A3AFE10}">
+      <formula1>"JUnit, UML"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD9B6EA-04DB-473D-9B8E-63793A2E9D42}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6599B5B9-7CBE-4FEE-B773-816B44F3DA60}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,10 +1642,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
         <v>1</v>
       </c>
       <c r="C1" s="3">
@@ -812,7 +1806,7 @@
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1318,26 +2312,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3A4903-353E-4552-8E0F-D25A39E4E38B}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD9B6EA-04DB-473D-9B8E-63793A2E9D42}">
-  <sheetPr>
-    <tabColor theme="9"/>
-  </sheetPr>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70DA23C-F50F-4DA4-95BF-7A4D1188C47D}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Test Design for Delivery Area
Added test design of Delivery Area
</commit_message>
<xml_diff>
--- a/Documents/Test Designs.xlsx
+++ b/Documents/Test Designs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captain\Documents\GitHub\SoftwareEngineeringGroup\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave1\OneDrive\Documents\GitHub\SoftwareEngineeringGroup\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DA652B-DAA1-4179-BBA7-FAC23267DC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93911502-45D0-493E-8261-8813D837F50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5A776C0D-4F55-48DC-9152-FD2EB1331C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26985" windowHeight="15600" activeTab="1" xr2:uid="{5A776C0D-4F55-48DC-9152-FD2EB1331C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="158">
   <si>
     <t>Test Number</t>
   </si>
@@ -409,6 +409,108 @@
   </si>
   <si>
     <t>"wervghjmki"</t>
+  </si>
+  <si>
+    <t>Test Type (UAT or JUNIT)</t>
+  </si>
+  <si>
+    <t>Test Procedure (For Junit)</t>
+  </si>
+  <si>
+    <t>Very valid delivery area ID (2 Digits)</t>
+  </si>
+  <si>
+    <t>deliveryAreaID = 11</t>
+  </si>
+  <si>
+    <t>"Delivery Area ID  entered successfully"</t>
+  </si>
+  <si>
+    <t>1. Run the program</t>
+  </si>
+  <si>
+    <t>3. Observed the output</t>
+  </si>
+  <si>
+    <t>Verify negative delivery area ID entered displays error message</t>
+  </si>
+  <si>
+    <t>deliveryAreaID = -13</t>
+  </si>
+  <si>
+    <t>Error Message: "Error, delivery area ID must be a positive number"</t>
+  </si>
+  <si>
+    <t>Verify negative delivery area ID digit count displays error message</t>
+  </si>
+  <si>
+    <t>Error message: "Error, delivery area ID must be 2 digits in length"</t>
+  </si>
+  <si>
+    <t>deliveryAreaID = 8, deliveryAreaID = 639</t>
+  </si>
+  <si>
+    <t>Error message: "Error, delivery area ID cannot be left empty"</t>
+  </si>
+  <si>
+    <t>deliveryAreaID = null</t>
+  </si>
+  <si>
+    <t>Verify delivery area ID empty input displays error message</t>
+  </si>
+  <si>
+    <t>Verify valid name of Delivery Area (2-50 characters)</t>
+  </si>
+  <si>
+    <t>Verify error message is displayed when name entered is lower than minimum characters allowed</t>
+  </si>
+  <si>
+    <t>deliveryAreaName = "Widgeborough"</t>
+  </si>
+  <si>
+    <t>deliveryAreaName = "F"</t>
+  </si>
+  <si>
+    <t>"Delivery Area name entered successfully"</t>
+  </si>
+  <si>
+    <t>Error message: "Error, delivery area name must be greater than 2 characters"</t>
+  </si>
+  <si>
+    <t>Verify error message is displayed when name entered is higher than the maximum characters allowed</t>
+  </si>
+  <si>
+    <t>deliveryAreaName = enter value greater than 50 characters</t>
+  </si>
+  <si>
+    <t>Error Message: "Error, delivery area name must be lower than 50 characters"</t>
+  </si>
+  <si>
+    <t>Verify empty delivery area name displays error message</t>
+  </si>
+  <si>
+    <t>deliveryAreaName = null</t>
+  </si>
+  <si>
+    <t>Error message: "Error, delivery area name cannot be empty"</t>
+  </si>
+  <si>
+    <t>deliveryAreaID = F39D</t>
+  </si>
+  <si>
+    <t>Verify delivery area ID alphabetical characters entered displays error message</t>
+  </si>
+  <si>
+    <t>Error message: "Error, delivery area ID cannot contain alphabetical characters"</t>
+  </si>
+  <si>
+    <t>Verify delivery area name numercial characters entered displays error message</t>
+  </si>
+  <si>
+    <t>deliveryAreaName = 82910383</t>
+  </si>
+  <si>
+    <t>Error message: "Error, delivery area ID cannot contain numerical characters"</t>
   </si>
 </sst>
 </file>
@@ -492,7 +594,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -528,26 +630,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -587,15 +674,24 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -934,7 +1030,7 @@
   </sheetPr>
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -1011,7 +1107,7 @@
       <c r="D4" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1028,15 +1124,15 @@
       <c r="D5" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="E5" s="14" t="b">
+      <c r="E5" s="13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1050,8 +1146,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" t="s">
         <v>70</v>
       </c>
       <c r="C7" t="s">
@@ -1065,8 +1161,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="23"/>
+      <c r="B8" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1075,7 +1171,7 @@
       <c r="D8" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1083,16 +1179,16 @@
       <c r="A9" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="25" t="b">
+      <c r="B9" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="18" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1160,7 +1256,7 @@
       <c r="D14" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1177,12 +1273,12 @@
       <c r="D15" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="E15" s="14" t="b">
+      <c r="E15" s="13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="22" t="s">
         <v>87</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -1199,7 +1295,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="23"/>
       <c r="B17" t="s">
         <v>70</v>
       </c>
@@ -1214,7 +1310,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="11" t="s">
         <v>71</v>
       </c>
@@ -1224,7 +1320,7 @@
       <c r="D18" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1232,16 +1328,16 @@
       <c r="A19" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="25" t="b">
+      <c r="B19" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="18" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1331,7 +1427,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="22" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -1348,7 +1444,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
+      <c r="A27" s="23"/>
       <c r="B27" t="s">
         <v>102</v>
       </c>
@@ -1363,14 +1459,14 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
+      <c r="A28" s="23"/>
       <c r="B28" t="s">
         <v>103</v>
       </c>
       <c r="C28" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" t="s">
         <v>109</v>
       </c>
       <c r="E28" t="s">
@@ -1378,24 +1474,24 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C29" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="26" t="b">
+      <c r="B29" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B31" s="6">
@@ -1412,7 +1508,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B32" t="s">
@@ -1480,7 +1576,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="21" t="s">
         <v>87</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -1497,7 +1593,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
+      <c r="A37" s="21"/>
       <c r="B37" t="s">
         <v>102</v>
       </c>
@@ -1512,7 +1608,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="27"/>
+      <c r="A38" s="21"/>
       <c r="B38" t="s">
         <v>115</v>
       </c>
@@ -1527,29 +1623,29 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="28" t="b">
+      <c r="B39" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="20" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="14" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1569,18 +1665,18 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="21" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="27"/>
+      <c r="A47" s="21"/>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="27"/>
+      <c r="A48" s="21"/>
     </row>
     <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="14" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1609,12 +1705,365 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+    <col min="3" max="3" width="87.5703125" customWidth="1"/>
+    <col min="4" max="4" width="93" customWidth="1"/>
+    <col min="5" max="5" width="64.5703125" customWidth="1"/>
+    <col min="6" max="6" width="75.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2</v>
+      </c>
+      <c r="D1" s="24">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="6">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6">
+        <v>9</v>
+      </c>
+      <c r="F11" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1626,8 +2075,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>